<commit_message>
updated f1 score graph excel
</commit_message>
<xml_diff>
--- a/assignment2/naive-base-topic-evaluation.xlsx
+++ b/assignment2/naive-base-topic-evaluation.xlsx
@@ -87,6 +87,275 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>F1 Score</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.26396728861488999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27501692690845803</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28702793023074702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30016774616366398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.31454162335654001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33034664701345201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34777965146240197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.367135025071262</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.38866057904310802</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41283939748341902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.440114623909034</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.47101523078346502</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.50618838833581203</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54594535636430896</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.59083970991062496</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.64107084900100997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68934221255390304</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.72478799833969498</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.69176873776451997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.514511760994524</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="56600256"/>
+        <c:axId val="137751360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="56600256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="137751360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="137751360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56600256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,7 +652,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,6 +831,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>